<commit_message>
added price to best western
</commit_message>
<xml_diff>
--- a/working_windows_extension/version_4/best_western/booking/Expenses.xlsx
+++ b/working_windows_extension/version_4/best_western/booking/Expenses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Confirmation Number</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Michael McIntyre</t>
   </si>
   <si>
+    <t>92.88 USD</t>
+  </si>
+  <si>
     <t>Checked in, but different date</t>
   </si>
   <si>
@@ -46,12 +49,18 @@
     <t>Aphea Solomon</t>
   </si>
   <si>
+    <t>391.64 USD</t>
+  </si>
+  <si>
     <t>710493592-01</t>
   </si>
   <si>
     <t>Taha Rana</t>
   </si>
   <si>
+    <t>87.82 USD</t>
+  </si>
+  <si>
     <t>Cancelled</t>
   </si>
   <si>
@@ -61,10 +70,16 @@
     <t>shila sheedfar</t>
   </si>
   <si>
+    <t>88.29 USD</t>
+  </si>
+  <si>
     <t>904325399-01</t>
   </si>
   <si>
     <t>adelina rivera</t>
+  </si>
+  <si>
+    <t>109 USD</t>
   </si>
 </sst>
 </file>
@@ -432,19 +447,25 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
         <v>1698794068</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -452,13 +473,16 @@
         <v>1321603314</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -466,13 +490,16 @@
         <v>1404705656</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -480,13 +507,16 @@
         <v>1579387030</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>